<commit_message>
Trailing stop loss code add
</commit_message>
<xml_diff>
--- a/Nifty/Testing.xlsx
+++ b/Nifty/Testing.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,37 +513,35 @@
       <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.994343946560047</v>
+        <v>3.966420224404872</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>46049.40069444444</v>
+        <v>46051.42638888889</v>
       </c>
       <c r="E2" t="n">
-        <v>25035.400390625</v>
+        <v>25211.650390625</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>46049.40138888889</v>
+        <v>46051.42847222222</v>
       </c>
       <c r="H2" t="n">
-        <v>25082.75</v>
+        <v>25216.44921875</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>189.1306255790114</v>
+        <v>19.03416892843961</v>
       </c>
       <c r="K2" t="n">
-        <v>0.001891306255790114</v>
+        <v>0.0001903416892843961</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -563,37 +561,35 @@
       <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3.986889155567246</v>
+        <v>3.966915519577988</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>46049.42708333334</v>
+        <v>46051.43333333333</v>
       </c>
       <c r="E3" t="n">
-        <v>25129.650390625</v>
+        <v>25213.30078125</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>46049.42777777778</v>
+        <v>46051.43402777778</v>
       </c>
       <c r="H3" t="n">
-        <v>25145.400390625</v>
+        <v>25189.599609375</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>62.79350420019182</v>
+        <v>-94.02054654312087</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0006267496664369716</v>
+        <v>-0.0009400265391917668</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -613,37 +609,35 @@
       <c r="A4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B4" t="n">
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>4.006342928383698</v>
+        <v>3.964216474650057</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>46049.46666666667</v>
+        <v>46051.43958333333</v>
       </c>
       <c r="E4" t="n">
-        <v>25023.30078125</v>
+        <v>25206.75</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>46049.46944444445</v>
+        <v>46051.44097222222</v>
       </c>
       <c r="H4" t="n">
-        <v>25034</v>
+        <v>25205</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>42.8647393782885</v>
+        <v>-6.937378830625676</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0004275702411736136</v>
+        <v>-6.942584823497643e-05</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -663,37 +657,35 @@
       <c r="A5" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.99364449657456</v>
+        <v>3.962935003977417</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>46049.49861111111</v>
+        <v>46051.45277777778</v>
       </c>
       <c r="E5" t="n">
-        <v>25113.599609375</v>
+        <v>25213.150390625</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>46049.50208333333</v>
+        <v>46051.45625</v>
       </c>
       <c r="H5" t="n">
-        <v>25129.099609375</v>
+        <v>25220.05078125</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>61.90148969691654</v>
+        <v>27.34579954892979</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0006171954734126012</v>
+        <v>0.0002736822062333667</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -713,37 +705,35 @@
       <c r="A6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B6" t="n">
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>3.99468554099828</v>
+        <v>3.955187989176426</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>46049.51597222222</v>
+        <v>46051.48888888889</v>
       </c>
       <c r="E6" t="n">
-        <v>25122.55078125</v>
+        <v>25269.44921875</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>46049.51736111111</v>
+        <v>46051.48958333334</v>
       </c>
       <c r="H6" t="n">
-        <v>25134.19921875</v>
+        <v>25251.94921875</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>46.53184485646489</v>
+        <v>-69.21578981057974</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0004636646016332025</v>
+        <v>-0.0006925358700344367</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -763,37 +753,35 @@
       <c r="A7" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B7" t="n">
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>4.001013185365785</v>
+        <v>3.953215203312296</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>46049.53819444445</v>
+        <v>46051.50208333333</v>
       </c>
       <c r="E7" t="n">
-        <v>25094.44921875</v>
+        <v>25264.55078125</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>46049.54236111111</v>
+        <v>46051.50416666667</v>
       </c>
       <c r="H7" t="n">
-        <v>25076.349609375</v>
+        <v>25262.44921875</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>-72.41677575933863</v>
+        <v>-8.307928825714043</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0007212594792267746</v>
+        <v>-8.318226269672833e-05</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -813,37 +801,35 @@
       <c r="A8" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>3.998900221208068</v>
+        <v>3.940378118721523</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>46049.54791666667</v>
+        <v>46051.55763888889</v>
       </c>
       <c r="E8" t="n">
-        <v>25089.599609375</v>
+        <v>25344.75</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>46049.55486111111</v>
+        <v>46051.55972222222</v>
       </c>
       <c r="H8" t="n">
-        <v>25098.05078125</v>
+        <v>25342.849609375</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>33.79539308040694</v>
+        <v>-7.4882576357777</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0003368396469684051</v>
+        <v>-7.498162834516264e-05</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -863,37 +849,35 @@
       <c r="A9" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B9" t="n">
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>4.007450770469841</v>
+        <v>3.939251190551578</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>46049.59236111111</v>
+        <v>46051.56319444445</v>
       </c>
       <c r="E9" t="n">
-        <v>25044.5</v>
+        <v>25350.099609375</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>46049.59444444445</v>
+        <v>46051.56944444445</v>
       </c>
       <c r="H9" t="n">
-        <v>25024.650390625</v>
+        <v>25384.650390625</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>-79.54633238336828</v>
+        <v>136.1042061735498</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0007925735940026667</v>
+        <v>0.001362944595185039</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -913,37 +897,35 @@
       <c r="A10" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B10" t="n">
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>4.004858303653684</v>
+        <v>3.934872160829566</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>46049.60416666666</v>
+        <v>46051.59305555555</v>
       </c>
       <c r="E10" t="n">
-        <v>25040.849609375</v>
+        <v>25412.900390625</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>46049.60972222222</v>
+        <v>46051.59375</v>
       </c>
       <c r="H10" t="n">
-        <v>25071</v>
+        <v>25408.19921875</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>120.7480422529334</v>
+        <v>-18.49851033420418</v>
       </c>
       <c r="K10" t="n">
-        <v>0.001204048229007055</v>
+        <v>-0.0001849915516424957</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -963,37 +945,35 @@
       <c r="A11" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B11" t="n">
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>3.968898950340256</v>
+        <v>3.93385792748978</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>46050.41736111111</v>
+        <v>46051.59513888889</v>
       </c>
       <c r="E11" t="n">
-        <v>25298.150390625</v>
+        <v>25414.75</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>46050.41875</v>
+        <v>46051.59652777778</v>
       </c>
       <c r="H11" t="n">
-        <v>25282.80078125</v>
+        <v>25401.849609375</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>-60.92104853657656</v>
+        <v>-50.74830392787408</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0006067482854671385</v>
+        <v>-0.0005075946300868888</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1013,37 +993,35 @@
       <c r="A12" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B12" t="n">
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>3.970147519498783</v>
+        <v>3.931265647769494</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>46050.43333333333</v>
+        <v>46051.60138888889</v>
       </c>
       <c r="E12" t="n">
-        <v>25274.849609375</v>
+        <v>25418.599609375</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>46050.43680555555</v>
+        <v>46051.60208333333</v>
       </c>
       <c r="H12" t="n">
-        <v>25246.5</v>
+        <v>25412.349609375</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>-112.5521313389181</v>
+        <v>-24.57041029856191</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.001121652940102366</v>
+        <v>-0.000245882939896323</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1063,37 +1041,35 @@
       <c r="A13" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B13" t="n">
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>3.964627617356594</v>
+        <v>3.947474990060236</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>46050.44236111111</v>
+        <v>46052.40138888889</v>
       </c>
       <c r="E13" t="n">
-        <v>25281.650390625</v>
+        <v>25308</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>46050.44375</v>
+        <v>46052.40208333333</v>
       </c>
       <c r="H13" t="n">
-        <v>25301.599609375</v>
+        <v>25290.650390625</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>79.0912236009317</v>
+        <v>-68.48714909513365</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0007890789739500562</v>
+        <v>-0.0006855385401849872</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1113,37 +1089,35 @@
       <c r="A14" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B14" t="n">
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>3.961566478107828</v>
+        <v>3.946523165993629</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>46050.49444444444</v>
+        <v>46052.40347222222</v>
       </c>
       <c r="E14" t="n">
-        <v>25321.150390625</v>
+        <v>25296.75</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>46050.50277777778</v>
+        <v>46052.40486111111</v>
       </c>
       <c r="H14" t="n">
-        <v>25328.75</v>
+        <v>25281.650390625</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>30.10635774671391</v>
+        <v>-59.59095819589857</v>
       </c>
       <c r="K14" t="n">
-        <v>0.000300128914277674</v>
+        <v>-0.0005968991817131309</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1163,37 +1137,35 @@
       <c r="A15" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B15" t="n">
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>3.969991174376801</v>
+        <v>3.942211592628031</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>46050.55069444444</v>
+        <v>46052.41736111111</v>
       </c>
       <c r="E15" t="n">
-        <v>25275</v>
+        <v>25309.30078125</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>46050.55277777778</v>
+        <v>46052.41944444444</v>
       </c>
       <c r="H15" t="n">
-        <v>25283.75</v>
+        <v>25288.599609375</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>34.73742277579731</v>
+        <v>-81.60839974660485</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0003461918892185984</v>
+        <v>-0.0008179274510157445</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1213,37 +1185,35 @@
       <c r="A16" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B16" t="n">
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>3.978440837294914</v>
+        <v>3.94034941781933</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>46050.58194444444</v>
+        <v>46052.42569444444</v>
       </c>
       <c r="E16" t="n">
-        <v>25230.05078125</v>
+        <v>25300.55078125</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>46050.59166666667</v>
+        <v>46052.42847222222</v>
       </c>
       <c r="H16" t="n">
-        <v>25210.69921875</v>
+        <v>25311.69921875</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>-76.98904651546036</v>
+        <v>43.9287392127153</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.000767004500616392</v>
+        <v>0.0004406401108176966</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1263,37 +1233,35 @@
       <c r="A17" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B17" t="n">
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>3.97532657619495</v>
+        <v>3.943426361408329</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>46050.59791666667</v>
+        <v>46052.44097222222</v>
       </c>
       <c r="E17" t="n">
-        <v>25230.44921875</v>
+        <v>25291.94921875</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>46050.60416666666</v>
+        <v>46052.44166666667</v>
       </c>
       <c r="H17" t="n">
-        <v>25249.099609375</v>
+        <v>25285.599609375</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>74.14139350797632</v>
+        <v>-25.03921699403145</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0007392016869497167</v>
+        <v>-0.0002510525906914106</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1313,37 +1281,35 @@
       <c r="A18" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B18" t="n">
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>3.981231499999937</v>
+        <v>3.942366027883426</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>46051.42638888889</v>
+        <v>46052.44305555556</v>
       </c>
       <c r="E18" t="n">
-        <v>25211.650390625</v>
+        <v>25292.400390625</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>46051.42777777778</v>
+        <v>46052.44583333333</v>
       </c>
       <c r="H18" t="n">
-        <v>25220.099609375</v>
+        <v>25296.05078125</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>33.63829583789629</v>
+        <v>14.39117598850862</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0003351315213042703</v>
+        <v>0.0001443275675152686</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1363,37 +1329,35 @@
       <c r="A19" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B19" t="n">
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>3.982305048795836</v>
+        <v>3.941073087397846</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>46051.43333333333</v>
+        <v>46052.45486111111</v>
       </c>
       <c r="E19" t="n">
-        <v>25213.30078125</v>
+        <v>25304.349609375</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>46051.43402777778</v>
+        <v>46052.45555555556</v>
       </c>
       <c r="H19" t="n">
-        <v>25189.599609375</v>
+        <v>25298.94921875</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>-94.38529642017966</v>
+        <v>-21.28333415363159</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0009400265391916796</v>
+        <v>-0.0002134174838859069</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1413,37 +1377,35 @@
       <c r="A20" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B20" t="n">
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>3.979595533004441</v>
+        <v>3.944479764145127</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>46051.43958333333</v>
+        <v>46052.47708333333</v>
       </c>
       <c r="E20" t="n">
-        <v>25206.75</v>
+        <v>25277.099609375</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>46051.44166666667</v>
+        <v>46052.47777777778</v>
       </c>
       <c r="H20" t="n">
-        <v>25219.94921875</v>
+        <v>25268.94921875</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>52.52755197664374</v>
+        <v>-32.14905089019157</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0005236382615767131</v>
+        <v>-0.0003224416863862554</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1463,37 +1425,35 @@
       <c r="A21" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B21" t="n">
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>3.980668647058683</v>
+        <v>3.94335598238643</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>46051.45277777778</v>
+        <v>46052.48611111111</v>
       </c>
       <c r="E21" t="n">
-        <v>25213.150390625</v>
+        <v>25276.150390625</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>46051.45347222222</v>
+        <v>46052.48819444444</v>
       </c>
       <c r="H21" t="n">
-        <v>25224.80078125</v>
+        <v>25272.05078125</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>46.37634468692704</v>
+        <v>-16.16621915435826</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0004620759581608154</v>
+        <v>-0.0001621927908975293</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1513,37 +1473,35 @@
       <c r="A22" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B22" t="n">
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>3.973635227621724</v>
+        <v>3.944175342901707</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>46051.48888888889</v>
+        <v>46052.49305555555</v>
       </c>
       <c r="E22" t="n">
-        <v>25269.44921875</v>
+        <v>25266.80078125</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>46051.48958333334</v>
+        <v>46052.49583333333</v>
       </c>
       <c r="H22" t="n">
-        <v>25251.94921875</v>
+        <v>25287.400390625</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>-69.53861648337625</v>
+        <v>81.24847137028701</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0006925358700344748</v>
+        <v>0.0008152836424897876</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -1563,37 +1521,35 @@
       <c r="A23" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B23" t="n">
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>3.971653240563786</v>
+        <v>3.946055846831565</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>46051.50208333333</v>
+        <v>46052.50694444445</v>
       </c>
       <c r="E23" t="n">
-        <v>25264.55078125</v>
+        <v>25275.349609375</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>46051.50625</v>
+        <v>46052.51180555556</v>
       </c>
       <c r="H23" t="n">
-        <v>25284.150390625</v>
+        <v>25287.349609375</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>77.84285208801157</v>
+        <v>47.35267016198486</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0007757750986630609</v>
+        <v>0.0004747708809357306</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -1613,37 +1569,35 @@
       <c r="A24" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B24" t="n">
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>3.962156968753998</v>
+        <v>3.944363506434533</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>46051.55763888889</v>
+        <v>46052.5375</v>
       </c>
       <c r="E24" t="n">
-        <v>25344.75</v>
+        <v>25298.19921875</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>46051.56388888889</v>
+        <v>46052.53819444445</v>
       </c>
       <c r="H24" t="n">
-        <v>25361</v>
+        <v>25292.69921875</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>64.38505074224668</v>
+        <v>-21.69399928538769</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0006411584253148497</v>
+        <v>-0.0002174067787371623</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -1663,37 +1617,35 @@
       <c r="A25" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B25" t="n">
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>3.954065114174827</v>
+        <v>3.942812244468532</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>46051.59305555555</v>
+        <v>46052.54097222222</v>
       </c>
       <c r="E25" t="n">
-        <v>25412.900390625</v>
+        <v>25302.650390625</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>46051.60277777778</v>
+        <v>46052.54166666666</v>
       </c>
       <c r="H25" t="n">
-        <v>25424.05078125</v>
+        <v>25287.349609375</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>44.08937057973526</v>
+        <v>-60.32810766242619</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0004387689108132513</v>
+        <v>-0.0006047106138599239</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -1713,37 +1665,35 @@
       <c r="A26" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B26" t="n">
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>3.972196627752089</v>
+        <v>3.9479719725214</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>46052.40138888889</v>
+        <v>46052.56527777778</v>
       </c>
       <c r="E26" t="n">
-        <v>25308</v>
+        <v>25254.30078125</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>46052.40208333333</v>
+        <v>46052.57361111111</v>
       </c>
       <c r="H26" t="n">
-        <v>25290.650390625</v>
+        <v>25302.349609375</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>-68.91605985218484</v>
+        <v>189.6954267499968</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.0006855385401848602</v>
+        <v>0.001902599820172945</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -1763,37 +1713,35 @@
       <c r="A27" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B27" t="n">
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>3.971238842748483</v>
+        <v>3.941351739558167</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>46052.40347222222</v>
+        <v>46052.61041666667</v>
       </c>
       <c r="E27" t="n">
-        <v>25296.75</v>
+        <v>25344.849609375</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>46052.40902777778</v>
+        <v>46052.61180555556</v>
       </c>
       <c r="H27" t="n">
-        <v>25305.55078125</v>
+        <v>25341.69921875</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>34.9500043465232</v>
+        <v>-12.41679757012753</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0003479016573274293</v>
+        <v>-0.0001243010186903485</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -1813,37 +1761,35 @@
       <c r="A28" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B28" t="n">
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>3.970650436700089</v>
+        <v>3.940325277071876</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>46052.41736111111</v>
+        <v>46052.61736111111</v>
       </c>
       <c r="E28" t="n">
-        <v>25309.30078125</v>
+        <v>25348.30078125</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>46052.41944444444</v>
+        <v>46052.61944444444</v>
       </c>
       <c r="H28" t="n">
-        <v>25288.599609375</v>
+        <v>25348.69921875</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>-82.19711714566802</v>
+        <v>1.569973352583474</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.0008179274510157566</v>
+        <v>1.571850923809299e-05</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -1863,37 +1809,35 @@
       <c r="A29" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B29" t="n">
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>3.968774828290026</v>
+        <v>3.873734878924628</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>46052.42569444444</v>
+        <v>46056.38541666666</v>
       </c>
       <c r="E29" t="n">
-        <v>25300.55078125</v>
+        <v>25784.44921875</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>46052.42638888889</v>
+        <v>46056.38611111111</v>
       </c>
       <c r="H29" t="n">
-        <v>25314.30078125</v>
+        <v>25780.099609375</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>54.57065388899355</v>
+        <v>-16.84923354562488</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0005434664296000793</v>
+        <v>-0.0001686911881691239</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -1913,37 +1857,35 @@
       <c r="A30" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B30" t="n">
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>3.972282202033968</v>
+        <v>3.874290805760008</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>46052.44097222222</v>
+        <v>46056.40902777778</v>
       </c>
       <c r="E30" t="n">
-        <v>25291.94921875</v>
+        <v>25776.400390625</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>46052.44375</v>
+        <v>46056.41111111111</v>
       </c>
       <c r="H30" t="n">
-        <v>25301.25</v>
+        <v>25774.5</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>36.9453278243891</v>
+        <v>-7.362665925786132</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0003677368307819333</v>
+        <v>-7.372598951753475e-05</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -1963,37 +1905,35 @@
       <c r="A31" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B31" t="n">
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>3.971795624692774</v>
+        <v>3.879717364646687</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>46052.45486111111</v>
+        <v>46056.42847222222</v>
       </c>
       <c r="E31" t="n">
-        <v>25304.349609375</v>
+        <v>25738.44921875</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>46052.4625</v>
+        <v>46056.43402777778</v>
       </c>
       <c r="H31" t="n">
-        <v>25287.80078125</v>
+        <v>25774.75</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>-65.72856314065575</v>
+        <v>140.8367713658663</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.000653991443386706</v>
+        <v>0.001410371733801104</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -2013,37 +1953,35 @@
       <c r="A32" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B32" t="n">
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>3.973477101930631</v>
+        <v>3.877641128137102</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>46052.47708333333</v>
+        <v>46056.45833333334</v>
       </c>
       <c r="E32" t="n">
-        <v>25277.099609375</v>
+        <v>25788.55078125</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>46052.47847222222</v>
+        <v>46056.46111111111</v>
       </c>
       <c r="H32" t="n">
-        <v>25258.94921875</v>
+        <v>25794</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>-72.12016153954028</v>
+        <v>21.13011474121595</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.000718056695803415</v>
+        <v>0.0002113037989696564</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
@@ -2063,37 +2001,35 @@
       <c r="A33" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B33" t="n">
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>3.970773032619624</v>
+        <v>3.878317736255779</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>46052.48611111111</v>
+        <v>46056.47083333333</v>
       </c>
       <c r="E33" t="n">
-        <v>25276.150390625</v>
+        <v>25789.5</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>46052.49166666667</v>
+        <v>46056.47152777778</v>
       </c>
       <c r="H33" t="n">
-        <v>25258.75</v>
+        <v>25776.849609375</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>-69.09300185079337</v>
+        <v>-49.06223433150444</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.0006884114216796582</v>
+        <v>-0.0004905248502297758</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
@@ -2113,37 +2049,35 @@
       <c r="A34" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B34" t="n">
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>3.969507821983906</v>
+        <v>3.876979068859231</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>46052.49305555555</v>
+        <v>46056.47291666667</v>
       </c>
       <c r="E34" t="n">
-        <v>25266.80078125</v>
+        <v>25785.75</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>46052.49444444444</v>
+        <v>46056.47916666666</v>
       </c>
       <c r="H34" t="n">
-        <v>25286.30078125</v>
+        <v>25807.650390625</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>77.40540252868959</v>
+        <v>84.90735605296504</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0007717637135316092</v>
+        <v>0.0008493214517708335</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -2163,37 +2097,35 @@
       <c r="A35" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B35" t="n">
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>3.971227709664573</v>
+        <v>3.871923173261454</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>46052.50694444445</v>
+        <v>46056.50902777778</v>
       </c>
       <c r="E35" t="n">
-        <v>25275.349609375</v>
+        <v>25841.349609375</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>46052.50902777778</v>
+        <v>46056.50972222222</v>
       </c>
       <c r="H35" t="n">
-        <v>25286</v>
+        <v>25836.55078125</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>42.29512636875734</v>
+        <v>-18.58069382168469</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0004213746116117425</v>
+        <v>-0.0001857034635396369</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
@@ -2213,37 +2145,35 @@
       <c r="A36" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B36" t="n">
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>3.969312716620311</v>
+        <v>3.877904643488554</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>46052.5375</v>
+        <v>46056.54166666666</v>
       </c>
       <c r="E36" t="n">
-        <v>25298.19921875</v>
+        <v>25796.69921875</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>46052.54236111111</v>
+        <v>46056.54375</v>
       </c>
       <c r="H36" t="n">
-        <v>25281.5</v>
+        <v>25799.400390625</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>-66.28442134200304</v>
+        <v>10.47488695691573</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.0006600951556118726</v>
+        <v>0.0001047099806100295</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
@@ -2263,37 +2193,35 @@
       <c r="A37" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B37" t="n">
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>3.973587719353575</v>
+        <v>3.878025012554116</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>46052.56527777778</v>
+        <v>46056.55486111111</v>
       </c>
       <c r="E37" t="n">
-        <v>25254.30078125</v>
+        <v>25798.599609375</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>46052.56805555556</v>
+        <v>46056.55555555555</v>
       </c>
       <c r="H37" t="n">
-        <v>25267.650390625</v>
+        <v>25793</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>53.04584387067007</v>
+        <v>-21.71542521678202</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0005286073643706688</v>
+        <v>-0.0002170509043043181</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -2313,37 +2241,35 @@
       <c r="A38" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B38" t="n">
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>3.961484358225118</v>
+        <v>3.878430887534623</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>46052.61041666667</v>
+        <v>46056.57083333333</v>
       </c>
       <c r="E38" t="n">
-        <v>25344.849609375</v>
+        <v>25790.30078125</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>46052.6125</v>
+        <v>46056.57430555556</v>
       </c>
       <c r="H38" t="n">
-        <v>25324.5</v>
+        <v>25799.25</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>-80.61465923505602</v>
+        <v>34.7089264193055</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.0008029090599722205</v>
+        <v>0.0003469993943035603</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
@@ -2363,37 +2289,35 @@
       <c r="A39" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B39" t="n">
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>3.957764723388484</v>
+        <v>3.882027192323072</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>46052.61736111111</v>
+        <v>46056.60972222222</v>
       </c>
       <c r="E39" t="n">
-        <v>25348.30078125</v>
+        <v>25775.349609375</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>46052.62361111111</v>
+        <v>46056.61041666667</v>
       </c>
       <c r="H39" t="n">
-        <v>25357.25</v>
+        <v>25766.5</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>35.41890227064141</v>
+        <v>-34.35442423517816</v>
       </c>
       <c r="K39" t="n">
-        <v>0.0003530500457301208</v>
+        <v>-0.0003433361529179374</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
@@ -2413,37 +2337,35 @@
       <c r="A40" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B40" t="n">
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>3.892192099227159</v>
+        <v>3.881951862886345</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>46056.38541666666</v>
+        <v>46056.62013888889</v>
       </c>
       <c r="E40" t="n">
-        <v>25784.44921875</v>
+        <v>25767</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>46056.3875</v>
+        <v>46056.62083333333</v>
       </c>
       <c r="H40" t="n">
-        <v>25795.30078125</v>
+        <v>25764</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>42.23636582677136</v>
+        <v>-11.64585558866384</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0004208568663979589</v>
+        <v>-0.000116427989288673</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
@@ -2463,37 +2385,35 @@
       <c r="A41" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B41" t="n">
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>3.895046025685009</v>
+        <v>3.885865664243066</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>46056.40902777778</v>
+        <v>46057.39027777778</v>
       </c>
       <c r="E41" t="n">
-        <v>25776.400390625</v>
+        <v>25738.05078125</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>46056.41180555556</v>
+        <v>46057.39444444444</v>
       </c>
       <c r="H41" t="n">
-        <v>25752</v>
+        <v>25769.80078125</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>-95.04064452907187</v>
+        <v>123.376234839714</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.0009466174584204369</v>
+        <v>0.001233582149240641</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
@@ -2513,37 +2433,35 @@
       <c r="A42" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B42" t="n">
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>3.897096689895744</v>
+        <v>3.885971397844747</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>46056.42847222222</v>
+        <v>46057.40347222222</v>
       </c>
       <c r="E42" t="n">
-        <v>25738.44921875</v>
+        <v>25769.099609375</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>46056.42916666667</v>
+        <v>46057.40763888889</v>
       </c>
       <c r="H42" t="n">
-        <v>25751.099609375</v>
+        <v>25787.5</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>49.29979543057561</v>
+        <v>71.50339167792117</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0004914977789642589</v>
+        <v>0.0007140486436827592</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
@@ -2563,37 +2481,35 @@
       <c r="A43" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B43" t="n">
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>3.891437169157848</v>
+        <v>3.886875760600486</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>46056.45833333334</v>
+        <v>46057.41597222222</v>
       </c>
       <c r="E43" t="n">
-        <v>25788.55078125</v>
+        <v>25781.5</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>46056.45902777778</v>
+        <v>46057.41666666666</v>
       </c>
       <c r="H43" t="n">
-        <v>25797.349609375</v>
+        <v>25778.5</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>34.24008681064879</v>
+        <v>-11.66062728180259</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0003411912596265536</v>
+        <v>-0.0001163625079999337</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
@@ -2613,37 +2529,35 @@
       <c r="A44" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B44" t="n">
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>3.892621614830903</v>
+        <v>3.891207844512715</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>46056.47083333333</v>
+        <v>46057.45</v>
       </c>
       <c r="E44" t="n">
-        <v>25789.5</v>
+        <v>25749.80078125</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>46056.475</v>
+        <v>46057.45277777778</v>
       </c>
       <c r="H44" t="n">
-        <v>25798.69921875</v>
+        <v>25750.349609375</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>35.80907774581283</v>
+        <v>2.135604305294692</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0003567040365265443</v>
+        <v>2.131387849031614e-05</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
@@ -2663,37 +2577,35 @@
       <c r="A45" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B45" t="n">
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>3.886196956872341</v>
+        <v>3.891835122831373</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>46056.50902777778</v>
+        <v>46057.45763888889</v>
       </c>
       <c r="E45" t="n">
-        <v>25841.349609375</v>
+        <v>25746.19921875</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>46056.51527777778</v>
+        <v>46057.45972222222</v>
       </c>
       <c r="H45" t="n">
-        <v>25824.75</v>
+        <v>25745.150390625</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>-64.5093514383916</v>
+        <v>-4.081866134685697</v>
       </c>
       <c r="K45" t="n">
-        <v>-0.0006423661931719329</v>
+        <v>-4.073720225995492e-05</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -2713,37 +2625,35 @@
       <c r="A46" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B46" t="n">
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>3.890422724665625</v>
+        <v>3.895307694365932</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>46056.54166666666</v>
+        <v>46057.4875</v>
       </c>
       <c r="E46" t="n">
-        <v>25796.69921875</v>
+        <v>25722.19921875</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>46056.54583333333</v>
+        <v>46057.48819444444</v>
       </c>
       <c r="H46" t="n">
-        <v>25810.099609375</v>
+        <v>25715.19921875</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>52.13318420689029</v>
+        <v>-27.26715386056458</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0005194614439377026</v>
+        <v>-0.0002721384723160914</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -2763,37 +2673,35 @@
       <c r="A47" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B47" t="n">
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>3.892156921948077</v>
+        <v>3.893626768600761</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>46056.55486111111</v>
+        <v>46057.49652777778</v>
       </c>
       <c r="E47" t="n">
-        <v>25798.599609375</v>
+        <v>25726.30078125</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>46056.55972222222</v>
+        <v>46057.49722222222</v>
       </c>
       <c r="H47" t="n">
-        <v>25764.55078125</v>
+        <v>25720.650390625</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>-132.52338207094</v>
+        <v>-22.00051219054149</v>
       </c>
       <c r="K47" t="n">
-        <v>-0.001319793657041259</v>
+        <v>-0.000219634788267568</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -2813,37 +2721,35 @@
       <c r="A48" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B48" t="n">
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>3.888270847039908</v>
+        <v>3.89046540815658</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>46056.57083333333</v>
+        <v>46057.52708333333</v>
       </c>
       <c r="E48" t="n">
-        <v>25790.30078125</v>
+        <v>25741.55078125</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>46056.57152777778</v>
+        <v>46057.52986111111</v>
       </c>
       <c r="H48" t="n">
-        <v>25799.099609375</v>
+        <v>25756.900390625</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>34.21222688654962</v>
+        <v>59.71712430214393</v>
       </c>
       <c r="K48" t="n">
-        <v>0.000341168108105052</v>
+        <v>0.0005962969949028137</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -2863,37 +2769,35 @@
       <c r="A49" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B49" t="n">
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>3.891853589234163</v>
+        <v>3.894071124441844</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>46056.60972222222</v>
+        <v>46057.54722222222</v>
       </c>
       <c r="E49" t="n">
-        <v>25775.349609375</v>
+        <v>25733.05078125</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>46056.61180555556</v>
+        <v>46057.54861111111</v>
       </c>
       <c r="H49" t="n">
-        <v>25749</v>
+        <v>25731.150390625</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>-102.5488218210085</v>
+        <v>-7.400256257969886</v>
       </c>
       <c r="K49" t="n">
-        <v>-0.001022279417130204</v>
+        <v>-7.385018749444284e-05</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -2913,37 +2817,35 @@
       <c r="A50" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B50" t="n">
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>3.889134865106162</v>
+        <v>3.886579317312464</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>46056.62013888889</v>
+        <v>46057.59097222222</v>
       </c>
       <c r="E50" t="n">
-        <v>25767</v>
+        <v>25780.75</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>46056.62430555555</v>
+        <v>46057.59652777778</v>
       </c>
       <c r="H50" t="n">
-        <v>25778.05078125</v>
+        <v>25806.19921875</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>42.97797864604217</v>
+        <v>98.91040723551123</v>
       </c>
       <c r="K50" t="n">
-        <v>0.0004288734136687031</v>
+        <v>0.0009871403566614693</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -2963,37 +2865,35 @@
       <c r="A51" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B51" t="n">
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>3.895179044439182</v>
+        <v>3.908631975435032</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>46057.39027777778</v>
+        <v>46058.42361111111</v>
       </c>
       <c r="E51" t="n">
-        <v>25738.05078125</v>
+        <v>25660.599609375</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>46057.39097222222</v>
+        <v>46058.42708333334</v>
       </c>
       <c r="H51" t="n">
-        <v>25751.30078125</v>
+        <v>25665.400390625</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>51.61112233881431</v>
+        <v>18.76448710080876</v>
       </c>
       <c r="K51" t="n">
-        <v>0.000514801999289367</v>
+        <v>0.0001870876488888999</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
@@ -3013,37 +2913,35 @@
       <c r="A52" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B52" t="n">
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>3.892488627491014</v>
+        <v>3.911093097425446</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>46057.40347222222</v>
+        <v>46058.46180555555</v>
       </c>
       <c r="E52" t="n">
-        <v>25769.099609375</v>
+        <v>25649.25</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>46057.40416666667</v>
+        <v>46058.46527777778</v>
       </c>
       <c r="H52" t="n">
-        <v>25778.849609375</v>
+        <v>25660.25</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>37.95176411804277</v>
+        <v>43.02202407168807</v>
       </c>
       <c r="K52" t="n">
-        <v>0.0003783601347271853</v>
+        <v>0.0004288624423716907</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
@@ -3063,37 +2961,35 @@
       <c r="A53" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B53" t="n">
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>3.892088471744987</v>
+        <v>3.910651074619181</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>46057.41597222222</v>
+        <v>46058.47916666666</v>
       </c>
       <c r="E53" t="n">
-        <v>25781.5</v>
+        <v>25663.150390625</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>46057.42222222222</v>
+        <v>46058.47986111111</v>
       </c>
       <c r="H53" t="n">
-        <v>25796.19921875</v>
+        <v>25658</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>57.21065984053712</v>
+        <v>-20.14138063236896</v>
       </c>
       <c r="K53" t="n">
-        <v>0.0005701459864632051</v>
+        <v>-0.0002006920641700542</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
@@ -3113,37 +3009,35 @@
       <c r="A54" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B54" t="n">
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>3.899101606535227</v>
+        <v>3.909630283111729</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>46057.45</v>
+        <v>46058.48333333333</v>
       </c>
       <c r="E54" t="n">
-        <v>25749.80078125</v>
+        <v>25664.69921875</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>46057.46041666667</v>
+        <v>46058.48888888889</v>
       </c>
       <c r="H54" t="n">
-        <v>25759.849609375</v>
+        <v>25666.30078125</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>39.18140188598773</v>
+        <v>6.261517250299221</v>
       </c>
       <c r="K54" t="n">
-        <v>0.0003902487716455714</v>
+        <v>6.240332241379742e-05</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -3163,37 +3057,35 @@
       <c r="A55" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B55" t="n">
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>3.904808843981145</v>
+        <v>3.911558209528734</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>46057.4875</v>
+        <v>46058.50347222222</v>
       </c>
       <c r="E55" t="n">
-        <v>25722.19921875</v>
+        <v>25653.650390625</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>46057.49097222222</v>
+        <v>46058.50486111111</v>
       </c>
       <c r="H55" t="n">
-        <v>25705.099609375</v>
+        <v>25640.400390625</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>-66.77070591611846</v>
+        <v>-51.82814627625339</v>
       </c>
       <c r="K55" t="n">
-        <v>-0.0006647802246447976</v>
+        <v>-0.0005164956954758201</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
@@ -3213,37 +3105,35 @@
       <c r="A56" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B56" t="n">
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>3.901590871675519</v>
+        <v>3.913687682106632</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>46057.49652777778</v>
+        <v>46058.53125</v>
       </c>
       <c r="E56" t="n">
-        <v>25726.30078125</v>
+        <v>25626.44921875</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>46057.50555555556</v>
+        <v>46058.53263888889</v>
       </c>
       <c r="H56" t="n">
-        <v>25735.19921875</v>
+        <v>25623.599609375</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>34.71806252218084</v>
+        <v>-11.1524811097479</v>
       </c>
       <c r="K56" t="n">
-        <v>0.0003458887298125224</v>
+        <v>-0.0001111979795044611</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
@@ -3263,37 +3153,35 @@
       <c r="A57" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B57" t="n">
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>3.900628179160159</v>
+        <v>3.911603864004261</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>46057.52708333333</v>
+        <v>46058.54027777778</v>
       </c>
       <c r="E57" t="n">
-        <v>25741.55078125</v>
+        <v>25637.25</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>46057.52847222222</v>
+        <v>46058.54444444444</v>
       </c>
       <c r="H57" t="n">
-        <v>25756.349609375</v>
+        <v>25637.69921875</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>57.72472600292531</v>
+        <v>1.75716579829168</v>
       </c>
       <c r="K57" t="n">
-        <v>0.0005749004110420573</v>
+        <v>1.752211138098576e-05</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
@@ -3313,37 +3201,35 @@
       <c r="A58" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B58" t="n">
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>3.904159826701616</v>
+        <v>3.911405410828875</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>46057.54722222222</v>
+        <v>46058.56875</v>
       </c>
       <c r="E58" t="n">
-        <v>25733.05078125</v>
+        <v>25639</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>46057.55694444444</v>
+        <v>46058.56944444445</v>
       </c>
       <c r="H58" t="n">
-        <v>25744.349609375</v>
+        <v>25634.400390625</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>44.11243085442402</v>
+        <v>-17.99093699707009</v>
       </c>
       <c r="K58" t="n">
-        <v>0.0004390784528832797</v>
+        <v>-0.000179398938141072</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
@@ -3363,37 +3249,35 @@
       <c r="A59" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>(7, 21, True, '^NSEI')</t>
-        </is>
+      <c r="B59" t="n">
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>3.898647460197369</v>
+        <v>3.915193283792673</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>46057.59097222222</v>
+        <v>46058.60277777778</v>
       </c>
       <c r="E59" t="n">
-        <v>25780.75</v>
+        <v>25609.599609375</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>46057.59236111111</v>
+        <v>46058.60416666666</v>
       </c>
       <c r="H59" t="n">
-        <v>25789.05078125</v>
+        <v>25607.650390625</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>32.3618197379692</v>
+        <v>-7.63156815864204</v>
       </c>
       <c r="K59" t="n">
-        <v>0.0003219759413516173</v>
+        <v>-7.611281627715339e-05</v>
       </c>
       <c r="L59" t="inlineStr">
         <is>
@@ -3407,6 +3291,342 @@
       </c>
       <c r="N59" t="n">
         <v>57</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>3.912931974891703</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>46058.61805555555</v>
+      </c>
+      <c r="E60" t="n">
+        <v>25622.44921875</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>46058.62847222222</v>
+      </c>
+      <c r="H60" t="n">
+        <v>25659.25</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>143.9989536541252</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.001436271019051186</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>3.927242493442983</v>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>46059.41041666667</v>
+      </c>
+      <c r="E61" t="n">
+        <v>25565.75</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>46059.41111111111</v>
+      </c>
+      <c r="H61" t="n">
+        <v>25560.75</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>-19.63621246721596</v>
+      </c>
+      <c r="K61" t="n">
+        <v>-0.0001955741568309267</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>3.92968700537708</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>46059.42986111111</v>
+      </c>
+      <c r="E62" t="n">
+        <v>25544.849609375</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>46059.43333333333</v>
+      </c>
+      <c r="H62" t="n">
+        <v>25544.69921875</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>-0.5909880847902969</v>
+      </c>
+      <c r="K62" t="n">
+        <v>-5.88731690728408e-06</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>3.933105008372531</v>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>46059.45763888889</v>
+      </c>
+      <c r="E63" t="n">
+        <v>25522.5</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>46059.46597222222</v>
+      </c>
+      <c r="H63" t="n">
+        <v>25563.599609375</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>161.6490794749698</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.001610328509158612</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>3.934097507699648</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>46059.54444444444</v>
+      </c>
+      <c r="E64" t="n">
+        <v>25557.150390625</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>46059.54652777778</v>
+      </c>
+      <c r="H64" t="n">
+        <v>25563.849609375</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>26.35537978791399</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.0002621269839402173</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>3.925521380120157</v>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>46059.59652777778</v>
+      </c>
+      <c r="E65" t="n">
+        <v>25619.69921875</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>46059.59861111111</v>
+      </c>
+      <c r="H65" t="n">
+        <v>25620</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>1.180723227618728</v>
+      </c>
+      <c r="K65" t="n">
+        <v>1.174023345992318e-05</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>3.925199702286681</v>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>46059.60694444444</v>
+      </c>
+      <c r="E66" t="n">
+        <v>25622.099609375</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>46059.61180555556</v>
+      </c>
+      <c r="H66" t="n">
+        <v>25639.69921875</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>69.08198147910298</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.0006868917709053836</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>